<commit_message>
... yet another minor edit...
</commit_message>
<xml_diff>
--- a/templates/2EXT04_DNA/2EXT04_DNA.xlsx
+++ b/templates/2EXT04_DNA/2EXT04_DNA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/2EXT04_DNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB6275-23CF-9048-9193-FCF0D21BABDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0927BF39-9C2D-D940-8D79-36ACEBCA5524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT04_DNA" sheetId="3" r:id="rId1"/>
@@ -930,7 +930,7 @@
       <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
minor edits in pairs of xlsx/json (to make swobup happy)
</commit_message>
<xml_diff>
--- a/templates/2EXT04_DNA/2EXT04_DNA.xlsx
+++ b/templates/2EXT04_DNA/2EXT04_DNA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/MetadataTemplates/SWATE_templates/templates/2EXT04_DNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97219A58-8635-9B41-B85C-AA19F43A978E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB40B43F-4FCF-FF4E-B2FA-CCDA5C7E477E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3900" yWindow="-20960" windowWidth="36580" windowHeight="20920" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
@@ -919,7 +919,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5EEB8C5-4C05-AA46-9FA8-0D61FE068A75}">
-  <dimension ref="A1:AB32"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="13" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
@@ -2059,21 +2059,21 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <customXml>
   <SwateTable Table="annotationTable1" Worksheet="2EXT04_DNA">
-    <TableValidation DateTime="2021-06-07 18:23" SwateVersion="0.4.7" TableName="annotationTable1" Userlist="" WorksheetName="2EXT04_DNA">
+    <TableValidation DateTime="2021-07-27 07:25" SwateVersion="0.4.7" TableName="annotationTable1" Userlist="" WorksheetName="2EXT04_DNA">
       <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="1" ColumnHeader="Sample Name" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="2" ColumnHeader="Parameter [Bio entity]" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="5" ColumnHeader="Parameter [Biosource amount]" Importance="None" Unit="milligram" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="5" ColumnHeader="Parameter [Biosource amount]" Importance="4" Unit="milligram" ValidationFormat="UnitTerm milligram"/>
       <ColumnValidation ColumnAdress="11" ColumnHeader="Parameter [Extraction method]" Importance="None" Unit="None" ValidationFormat="None"/>
       <ColumnValidation ColumnAdress="14" ColumnHeader="Parameter [Extraction buffer]" Importance="None" Unit="None" ValidationFormat="None"/>
-      <ColumnValidation ColumnAdress="17" ColumnHeader="Parameter [Extraction buffer volume]" Importance="None" Unit="microliter" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="17" ColumnHeader="Parameter [Extraction buffer volume]" Importance="4" Unit="microliter" ValidationFormat="UnitTerm microliter"/>
     </TableValidation>
   </SwateTable>
 </customXml>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C37A85D-7427-B341-B7C7-FCB2A04B0A2A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{735A6B34-FF92-0C46-8B30-B7D2C833FC29}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>